<commit_message>
Arreglos en el menu.
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>No</t>
   </si>
@@ -96,6 +96,33 @@
   </si>
   <si>
     <t>Jez Humble</t>
+  </si>
+  <si>
+    <t>El que se duerme pierde</t>
+  </si>
+  <si>
+    <t>Tom Peter</t>
+  </si>
+  <si>
+    <t>Sin lugar a duda</t>
+  </si>
+  <si>
+    <t>Ana Gutierrez</t>
+  </si>
+  <si>
+    <t>El arte de dormir</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Buscando a Nemo</t>
+  </si>
+  <si>
+    <t>Humble Po</t>
+  </si>
+  <si>
+    <t>Jose Ramirez</t>
   </si>
 </sst>
 </file>
@@ -422,8 +449,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -492,8 +519,8 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5">
-        <v>102</v>
+      <c r="D5" t="n">
+        <v>432.0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -504,7 +531,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>52</v>
@@ -577,6 +604,118 @@
         <v>23</v>
       </c>
       <c r="D11" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="n">
         <v>41.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Union parte C con parte B
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="32">
   <si>
     <t>No</t>
   </si>
@@ -887,6 +887,118 @@
         <v>41.0</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>